<commit_message>
updated files to reflect 2020-2021 new protocols; updated .md
</commit_message>
<xml_diff>
--- a/raw data/substrate_surfaceareas.xlsx
+++ b/raw data/substrate_surfaceareas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thell\Documents\Duke University\Research\HBEF\FieldExperiments\Summer2019\HB_chla_summer2019\data\tidy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thell\Documents\Duke University\Research\_HBEF\chla\hbef_chla\raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5833B963-DB48-4576-9C86-8E2E1BF7D989}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6432D6AE-6A2A-4970-B553-1932FEC78361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="2688" windowWidth="16416" windowHeight="9420" xr2:uid="{9D70326E-081A-4744-968B-CA6CF966C504}"/>
+    <workbookView xWindow="864" yWindow="-108" windowWidth="22284" windowHeight="13176" xr2:uid="{9D70326E-081A-4744-968B-CA6CF966C504}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -466,13 +468,13 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57" bestFit="1" customWidth="1"/>
@@ -577,8 +579,8 @@
         <v>1.8940000000000002E-2</v>
       </c>
       <c r="C6">
-        <f>0.0011584+(4*B6*0.024)</f>
-        <v>2.97664E-3</v>
+        <f>0.0011584+(4*B6*0.0254)</f>
+        <v>3.0827040000000003E-3</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>

</xml_diff>